<commit_message>
1. Correct missing features 2. Add percentage bar 3.Split into phases matching case clean up phases
Change-Id: I5db9e1d145137285c9fa81c2b15e95ed583e55f7
Reviewed-on: https://gerrit.dechocorp.com/47424
Reviewed-by: Leong He <leongh@mozy.com>
</commit_message>
<xml_diff>
--- a/automation_tracking.xlsx
+++ b/automation_tracking.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="540" windowWidth="23320" windowHeight="12500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16620" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="4" r:id="rId1"/>
     <sheet name="Automation Coverage" sheetId="1" r:id="rId2"/>
     <sheet name="Test Case Detail" sheetId="2" r:id="rId3"/>
     <sheet name="Add New Partner Detail" sheetId="3" r:id="rId4"/>
-    <sheet name="Plan" sheetId="5" r:id="rId5"/>
+    <sheet name="Overview" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4201" uniqueCount="874">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4192" uniqueCount="886">
   <si>
     <t>Billing Automation Test Plan</t>
   </si>
@@ -2579,27 +2579,12 @@
     <t>Bugs found in QA durring .36 testing</t>
   </si>
   <si>
-    <t>Total Cases</t>
-  </si>
-  <si>
-    <t>Automation Candidates</t>
-  </si>
-  <si>
-    <t>Complete Cases</t>
-  </si>
-  <si>
     <t>Note</t>
   </si>
   <si>
-    <t>Complete</t>
-  </si>
-  <si>
     <t>Leong</t>
   </si>
   <si>
-    <t>Pending</t>
-  </si>
-  <si>
     <t>Feature Name</t>
   </si>
   <si>
@@ -2690,12 +2675,6 @@
     <t>User Storage Details</t>
   </si>
   <si>
-    <t>Owner</t>
-  </si>
-  <si>
-    <t>Wait for BUS 2.5 Release</t>
-  </si>
-  <si>
     <t>Client Controller</t>
   </si>
   <si>
@@ -2715,17 +2694,75 @@
   </si>
   <si>
     <t>CongShan</t>
+  </si>
+  <si>
+    <t>Total Test Case #</t>
+  </si>
+  <si>
+    <t>Automation Candidate #</t>
+  </si>
+  <si>
+    <t>Completion %</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Automated Case #</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>Feature changed in 2.5</t>
+  </si>
+  <si>
+    <t>Rob clean up cases in progress</t>
+  </si>
+  <si>
+    <t>Automation Owner</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>Restrict Client to Limited Partners</t>
+  </si>
+  <si>
+    <t>Neale clean up cases in progress</t>
+  </si>
+  <si>
+    <t>Cleaning up cases</t>
+  </si>
+  <si>
+    <t>Phase I</t>
+  </si>
+  <si>
+    <t>Smoke Test (for production)</t>
+  </si>
+  <si>
+    <t>Phase II</t>
+  </si>
+  <si>
+    <t>Phase III</t>
+  </si>
+  <si>
+    <t>Phase IV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-409]mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="168" formatCode="00000"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2815,8 +2852,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2874,8 +2919,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -2898,8 +2949,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="94">
+  <cellStyleXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -2994,8 +3080,32 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
@@ -3017,9 +3127,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="6" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3029,12 +3136,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="94">
+  <cellStyles count="118">
     <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
     <cellStyle name="20% - Accent2" xfId="5" builtinId="34"/>
     <cellStyle name="20% - Accent3" xfId="6" builtinId="38"/>
@@ -3083,6 +3211,18 @@
     <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
@@ -3126,70 +3266,282 @@
     <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
         <right/>
-        <top/>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
         <bottom/>
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
         <bottom/>
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
         <bottom/>
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
         <bottom/>
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
         <bottom/>
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
         <bottom/>
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
-        <right/>
-        <top/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
@@ -3199,12 +3551,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -3237,22 +3583,25 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B2:H52" totalsRowCount="1" headerRowDxfId="11">
-  <autoFilter ref="B2:H51"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B2:H59" totalsRowCount="1" headerRowDxfId="8">
+  <autoFilter ref="B2:H58"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Feature Name" totalsRowLabel="Total" totalsRowDxfId="6"/>
-    <tableColumn id="2" name="Total Cases" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="5">
-      <totalsRowFormula>SUM(Table13[Total Cases])</totalsRowFormula>
+    <tableColumn id="2" name="Total Test Case #" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="5">
+      <totalsRowFormula>SUM(Table13[Total Test Case '#])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="Automation Candidates" totalsRowFunction="custom" dataDxfId="8" totalsRowDxfId="4">
-      <totalsRowFormula>SUM(Table13[Automation Candidates])</totalsRowFormula>
+    <tableColumn id="6" name="Automation Candidate #" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="4">
+      <totalsRowFormula>SUM(Table13[Automation Candidate '#])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" name="Complete Cases" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="3">
-      <totalsRowFormula>SUM(Table13[Complete Cases])</totalsRowFormula>
+    <tableColumn id="10" name="Automated Case #" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="3">
+      <totalsRowFormula>SUM(Table13[Automated Case '#])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="Status" totalsRowDxfId="2"/>
-    <tableColumn id="7" name="Owner" dataDxfId="10" totalsRowDxfId="1"/>
-    <tableColumn id="11" name="Note" totalsRowDxfId="0"/>
+    <tableColumn id="3" name="Completion %" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="2">
+      <calculatedColumnFormula>IF(AND(D3=0,D3&lt;&gt;""),100,IF(ISERROR(E3/D3*100),0,ROUNDUP(E3/D3 * 100, 0)))</calculatedColumnFormula>
+      <totalsRowFormula>ROUNDUP(E59/D59 * 100, 0)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="7" name="Automation Owner" dataDxfId="10" totalsRowDxfId="1"/>
+    <tableColumn id="11" name="Note" dataDxfId="9" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3547,7 +3896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
@@ -4617,7 +4966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView topLeftCell="A141" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -5496,7 +5845,7 @@
   <dimension ref="A1:P702"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D98" sqref="D98"/>
     </sheetView>
   </sheetViews>
@@ -20405,19 +20754,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:19">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>685</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
       <c r="L2" t="s">
         <v>686</v>
       </c>
@@ -21687,834 +22036,1164 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H52"/>
+  <dimension ref="A2:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" style="19" customWidth="1"/>
+    <col min="4" max="5" width="11.1640625" style="19" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" style="19" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" style="27" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="28">
+    <row r="2" spans="1:8" ht="28">
       <c r="B2" s="20" t="s">
+        <v>830</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>867</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>868</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>872</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>869</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>876</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="29" t="s">
+        <v>881</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>831</v>
+      </c>
+      <c r="C3" s="19">
+        <v>37</v>
+      </c>
+      <c r="D3" s="20">
+        <v>37</v>
+      </c>
+      <c r="E3" s="20">
+        <v>37</v>
+      </c>
+      <c r="F3" s="20">
+        <f t="shared" ref="F3:F34" si="0">IF(AND(D3=0,D3&lt;&gt;""),100,IF(ISERROR(E3/D3*100),0,ROUNDUP(E3/D3 * 100, 0)))</f>
+        <v>100</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>794</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="29"/>
+      <c r="B4" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="19">
+        <v>35</v>
+      </c>
+      <c r="D4" s="20">
+        <v>35</v>
+      </c>
+      <c r="E4" s="20">
+        <v>35</v>
+      </c>
+      <c r="F4" s="20">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>794</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="29"/>
+      <c r="B5" s="21" t="s">
+        <v>687</v>
+      </c>
+      <c r="C5" s="19">
+        <v>17</v>
+      </c>
+      <c r="D5" s="20">
+        <v>17</v>
+      </c>
+      <c r="E5" s="20">
+        <v>17</v>
+      </c>
+      <c r="F5" s="20">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>794</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="29"/>
+      <c r="B6" s="21" t="s">
+        <v>832</v>
+      </c>
+      <c r="C6" s="19">
+        <v>1</v>
+      </c>
+      <c r="D6" s="20">
+        <v>1</v>
+      </c>
+      <c r="E6" s="20">
+        <v>1</v>
+      </c>
+      <c r="F6" s="20">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>794</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="29"/>
+      <c r="B7" s="21" t="s">
+        <v>833</v>
+      </c>
+      <c r="C7" s="19">
+        <v>1</v>
+      </c>
+      <c r="D7" s="20">
+        <v>1</v>
+      </c>
+      <c r="E7" s="20">
+        <v>1</v>
+      </c>
+      <c r="F7" s="20">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>794</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="29"/>
+      <c r="B8" s="21" t="s">
+        <v>834</v>
+      </c>
+      <c r="C8" s="19">
+        <v>9</v>
+      </c>
+      <c r="D8" s="20">
+        <v>9</v>
+      </c>
+      <c r="E8" s="20">
+        <v>9</v>
+      </c>
+      <c r="F8" s="20">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>794</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="29"/>
+      <c r="B9" s="21" t="s">
         <v>835</v>
       </c>
-      <c r="C2" s="20" t="s">
-        <v>828</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>829</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>830</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>865</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8">
-      <c r="B3" s="22" t="s">
-        <v>836</v>
-      </c>
-      <c r="C3" s="20">
-        <v>37</v>
-      </c>
-      <c r="D3" s="21">
-        <v>37</v>
-      </c>
-      <c r="E3" s="21">
-        <v>37</v>
-      </c>
-      <c r="F3" t="s">
-        <v>832</v>
-      </c>
-      <c r="G3" s="20" t="s">
+      <c r="C9" s="19">
+        <v>74</v>
+      </c>
+      <c r="D9" s="20">
+        <v>74</v>
+      </c>
+      <c r="E9" s="20">
+        <v>74</v>
+      </c>
+      <c r="F9" s="20">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G9" s="19" t="s">
         <v>794</v>
       </c>
-      <c r="H3" s="20"/>
-    </row>
-    <row r="4" spans="2:8">
-      <c r="B4" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="20">
-        <v>35</v>
-      </c>
-      <c r="D4" s="21">
-        <v>35</v>
-      </c>
-      <c r="E4" s="21">
-        <v>35</v>
-      </c>
-      <c r="F4" t="s">
-        <v>832</v>
-      </c>
-      <c r="G4" s="20" t="s">
+      <c r="H9" s="19" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="29"/>
+      <c r="B10" s="21" t="s">
+        <v>856</v>
+      </c>
+      <c r="C10" s="19">
+        <v>24</v>
+      </c>
+      <c r="D10" s="20">
+        <v>24</v>
+      </c>
+      <c r="E10" s="20">
+        <v>24</v>
+      </c>
+      <c r="F10" s="20">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G10" s="19" t="s">
         <v>794</v>
       </c>
-      <c r="H4" s="20"/>
-    </row>
-    <row r="5" spans="2:8">
-      <c r="B5" s="22" t="s">
-        <v>687</v>
-      </c>
-      <c r="C5" s="20">
-        <v>17</v>
-      </c>
-      <c r="D5" s="21">
-        <v>17</v>
-      </c>
-      <c r="E5" s="21">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>832</v>
-      </c>
-      <c r="G5" s="20" t="s">
+      <c r="H10" s="19" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="29"/>
+      <c r="B11" s="21" t="s">
+        <v>857</v>
+      </c>
+      <c r="C11" s="19">
+        <v>12</v>
+      </c>
+      <c r="D11" s="20">
+        <v>12</v>
+      </c>
+      <c r="E11" s="20">
+        <v>12</v>
+      </c>
+      <c r="F11" s="20">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G11" s="19" t="s">
         <v>794</v>
       </c>
-      <c r="H5" s="20"/>
-    </row>
-    <row r="6" spans="2:8">
-      <c r="B6" s="22" t="s">
-        <v>837</v>
-      </c>
-      <c r="C6" s="20">
-        <v>1</v>
-      </c>
-      <c r="D6" s="21">
-        <v>1</v>
-      </c>
-      <c r="E6" s="21">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
-        <v>832</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>794</v>
-      </c>
-      <c r="H6" s="20"/>
-    </row>
-    <row r="7" spans="2:8">
-      <c r="B7" s="22" t="s">
-        <v>838</v>
-      </c>
-      <c r="C7" s="20">
-        <v>1</v>
-      </c>
-      <c r="D7" s="21">
-        <v>1</v>
-      </c>
-      <c r="E7" s="21">
-        <v>1</v>
-      </c>
-      <c r="F7" t="s">
-        <v>832</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>794</v>
-      </c>
-      <c r="H7" s="20"/>
-    </row>
-    <row r="8" spans="2:8">
-      <c r="B8" s="22" t="s">
-        <v>839</v>
-      </c>
-      <c r="C8" s="20">
-        <v>9</v>
-      </c>
-      <c r="D8" s="21">
-        <v>9</v>
-      </c>
-      <c r="E8" s="21">
-        <v>9</v>
-      </c>
-      <c r="F8" t="s">
-        <v>832</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>794</v>
-      </c>
-      <c r="H8" s="20"/>
-    </row>
-    <row r="9" spans="2:8">
-      <c r="B9" s="22" t="s">
-        <v>840</v>
-      </c>
-      <c r="C9" s="20">
-        <v>74</v>
-      </c>
-      <c r="D9" s="21">
-        <v>74</v>
-      </c>
-      <c r="E9" s="21">
-        <v>74</v>
-      </c>
-      <c r="F9" t="s">
-        <v>832</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>794</v>
-      </c>
-      <c r="H9" s="20"/>
-    </row>
-    <row r="10" spans="2:8">
-      <c r="B10" s="22" t="s">
-        <v>861</v>
-      </c>
-      <c r="C10" s="20">
-        <v>24</v>
-      </c>
-      <c r="D10" s="21">
-        <v>24</v>
-      </c>
-      <c r="E10" s="21">
-        <v>24</v>
-      </c>
-      <c r="F10" t="s">
-        <v>832</v>
-      </c>
-      <c r="G10" s="20" t="s">
-        <v>794</v>
-      </c>
-      <c r="H10" s="20"/>
-    </row>
-    <row r="11" spans="2:8">
-      <c r="B11" s="22" t="s">
-        <v>862</v>
-      </c>
-      <c r="C11" s="20">
-        <v>12</v>
-      </c>
-      <c r="D11" s="21">
-        <v>12</v>
-      </c>
-      <c r="E11" s="21">
-        <v>12</v>
-      </c>
-      <c r="F11" t="s">
-        <v>832</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>794</v>
-      </c>
-      <c r="H11" s="20"/>
-    </row>
-    <row r="12" spans="2:8">
-      <c r="B12" s="22" t="s">
-        <v>863</v>
-      </c>
-      <c r="C12" s="20">
+      <c r="H11" s="19" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="29"/>
+      <c r="B12" s="21" t="s">
+        <v>858</v>
+      </c>
+      <c r="C12" s="19">
         <v>14</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="20">
         <v>14</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="20">
         <v>14</v>
       </c>
-      <c r="F12" t="s">
-        <v>832</v>
-      </c>
-      <c r="G12" s="20" t="s">
+      <c r="F12" s="20">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G12" s="19" t="s">
         <v>796</v>
       </c>
-      <c r="H12" s="20"/>
-    </row>
-    <row r="13" spans="2:8">
-      <c r="B13" s="22" t="s">
-        <v>864</v>
-      </c>
-      <c r="C13" s="20">
+      <c r="H12" s="19" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="29"/>
+      <c r="B13" s="21" t="s">
+        <v>859</v>
+      </c>
+      <c r="C13" s="19">
         <v>29</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="20">
         <v>29</v>
       </c>
-      <c r="E13" s="21">
+      <c r="E13" s="20">
         <v>29</v>
       </c>
-      <c r="F13" t="s">
-        <v>832</v>
-      </c>
-      <c r="G13" s="20" t="s">
+      <c r="F13" s="20">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G13" s="19" t="s">
         <v>796</v>
       </c>
-      <c r="H13" s="20"/>
-    </row>
-    <row r="14" spans="2:8">
+      <c r="H13" s="19" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="29"/>
       <c r="B14" t="s">
         <v>817</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="19">
         <v>3</v>
       </c>
-      <c r="D14" s="20">
+      <c r="D14" s="19">
         <v>3</v>
       </c>
-      <c r="E14" s="20">
+      <c r="E14" s="19">
         <v>3</v>
       </c>
-      <c r="F14" t="s">
-        <v>832</v>
-      </c>
-      <c r="G14" s="20" t="s">
+      <c r="F14" s="20">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G14" s="19" t="s">
         <v>794</v>
       </c>
-    </row>
-    <row r="15" spans="2:8">
+      <c r="H14" s="19" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="29"/>
       <c r="B15" t="s">
         <v>821</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="19">
         <v>26</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D15" s="19">
         <v>0</v>
       </c>
-      <c r="E15" s="20">
+      <c r="E15" s="19">
         <v>0</v>
       </c>
-      <c r="F15" t="s">
-        <v>832</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8">
+      <c r="F15" s="20">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>870</v>
+      </c>
+      <c r="H15" s="19" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="29"/>
       <c r="B16" t="s">
-        <v>822</v>
-      </c>
-      <c r="C16" s="20">
-        <v>20</v>
-      </c>
-      <c r="D16" s="20">
+        <v>819</v>
+      </c>
+      <c r="C16" s="19">
+        <v>3</v>
+      </c>
+      <c r="D16" s="19">
         <v>0</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E16" s="19">
         <v>0</v>
       </c>
-      <c r="F16" t="s">
-        <v>832</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8">
+      <c r="F16" s="20">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>870</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="29"/>
       <c r="B17" t="s">
-        <v>819</v>
-      </c>
-      <c r="C17" s="20">
-        <v>3</v>
-      </c>
-      <c r="D17" s="20">
+        <v>863</v>
+      </c>
+      <c r="C17" s="19">
+        <v>2</v>
+      </c>
+      <c r="D17" s="19">
+        <v>2</v>
+      </c>
+      <c r="E17" s="19">
+        <v>2</v>
+      </c>
+      <c r="F17" s="20">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>796</v>
+      </c>
+      <c r="H17" s="27" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="29"/>
+      <c r="B18" t="s">
+        <v>864</v>
+      </c>
+      <c r="C18" s="19">
+        <v>1</v>
+      </c>
+      <c r="D18" s="19">
         <v>0</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E18" s="19">
         <v>0</v>
       </c>
-      <c r="F17" t="s">
-        <v>832</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8">
-      <c r="B18" t="s">
+      <c r="F18" s="20">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>870</v>
+      </c>
+      <c r="H18" s="27" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="29"/>
+      <c r="B19" t="s">
         <v>818</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C19" s="19">
         <v>17</v>
       </c>
-      <c r="D18" s="20">
+      <c r="D19" s="19">
         <v>13</v>
       </c>
-      <c r="E18" s="20">
-        <v>2</v>
-      </c>
-      <c r="F18" t="s">
-        <v>751</v>
-      </c>
-      <c r="G18" s="20" t="s">
+      <c r="E19" s="19">
+        <v>6</v>
+      </c>
+      <c r="F19" s="20">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="G19" s="19" t="s">
         <v>794</v>
       </c>
-    </row>
-    <row r="19" spans="2:8">
-      <c r="B19" t="s">
+      <c r="H19" s="27" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="29"/>
+      <c r="B20" t="s">
         <v>820</v>
       </c>
-      <c r="C19" s="20">
+      <c r="C20" s="19">
         <v>23</v>
       </c>
-      <c r="D19" s="20">
+      <c r="D20" s="19">
         <v>16</v>
       </c>
-      <c r="E19" s="20">
+      <c r="E20" s="19">
         <v>0</v>
       </c>
-      <c r="F19" t="s">
-        <v>751</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>833</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8">
-      <c r="B20" t="s">
-        <v>872</v>
-      </c>
-      <c r="C20" s="20">
+      <c r="F20" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>829</v>
+      </c>
+      <c r="H20" s="27" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="29"/>
+      <c r="B21" t="s">
+        <v>865</v>
+      </c>
+      <c r="C21" s="19">
         <v>1</v>
       </c>
-      <c r="D20" s="20">
+      <c r="D21" s="19">
         <v>1</v>
       </c>
-      <c r="E20" s="20">
+      <c r="E21" s="19">
         <v>0</v>
       </c>
-      <c r="F20" t="s">
-        <v>751</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>833</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8">
-      <c r="B21" t="s">
+      <c r="F21" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>829</v>
+      </c>
+      <c r="H21" s="27" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="29"/>
+      <c r="B22" t="s">
         <v>825</v>
       </c>
-      <c r="C21" s="20">
+      <c r="C22" s="19">
         <v>7</v>
       </c>
-      <c r="D21" s="20">
+      <c r="D22" s="19">
         <v>7</v>
       </c>
-      <c r="E21" s="20">
+      <c r="E22" s="19">
         <v>1</v>
       </c>
-      <c r="F21" t="s">
-        <v>751</v>
-      </c>
-      <c r="G21" s="20" t="s">
+      <c r="F22" s="20">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>866</v>
+      </c>
+      <c r="H22" s="27" t="s">
         <v>873</v>
       </c>
     </row>
-    <row r="22" spans="2:8">
-      <c r="B22" t="s">
+    <row r="23" spans="1:8">
+      <c r="A23" s="29"/>
+      <c r="B23" t="s">
         <v>826</v>
       </c>
-      <c r="C22" s="20">
+      <c r="C23" s="19">
         <v>34</v>
       </c>
-      <c r="D22" s="20">
+      <c r="D23" s="19">
         <v>15</v>
       </c>
-      <c r="E22" s="20">
+      <c r="E23" s="19">
         <v>0</v>
       </c>
-      <c r="F22" t="s">
-        <v>751</v>
-      </c>
-      <c r="G22" s="20" t="s">
+      <c r="F23" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="19" t="s">
+        <v>866</v>
+      </c>
+      <c r="H23" s="27" t="s">
         <v>873</v>
       </c>
     </row>
-    <row r="23" spans="2:8">
-      <c r="B23" t="s">
+    <row r="24" spans="1:8">
+      <c r="A24" s="29"/>
+      <c r="B24" t="s">
         <v>827</v>
       </c>
-      <c r="C23" s="20">
+      <c r="C24" s="19">
         <v>21</v>
       </c>
-      <c r="D23" s="20">
+      <c r="D24" s="19">
         <v>5</v>
       </c>
-      <c r="E23" s="20">
+      <c r="E24" s="19">
         <v>0</v>
       </c>
-      <c r="F23" t="s">
-        <v>751</v>
-      </c>
-      <c r="G23" s="20" t="s">
-        <v>833</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8">
-      <c r="B24" s="22" t="s">
-        <v>841</v>
-      </c>
-      <c r="C24" s="20">
-        <v>293</v>
-      </c>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21">
-        <v>18</v>
-      </c>
-      <c r="F24" t="s">
-        <v>751</v>
-      </c>
-      <c r="G24" s="20" t="s">
-        <v>794</v>
-      </c>
-      <c r="H24" s="20"/>
-    </row>
-    <row r="25" spans="2:8">
+      <c r="F24" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="19" t="s">
+        <v>829</v>
+      </c>
+      <c r="H24" s="27" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="29"/>
       <c r="B25" t="s">
         <v>823</v>
       </c>
-      <c r="C25" s="20">
+      <c r="C25" s="19">
         <v>124</v>
       </c>
-      <c r="D25" s="20">
+      <c r="D25" s="19">
         <v>105</v>
       </c>
-      <c r="E25" s="20">
+      <c r="E25" s="19">
         <v>0</v>
       </c>
-      <c r="F25" t="s">
-        <v>834</v>
-      </c>
-      <c r="H25" t="s">
-        <v>866</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8">
+      <c r="F25" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="27" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="29"/>
       <c r="B26" t="s">
         <v>824</v>
       </c>
-      <c r="C26" s="20">
+      <c r="C26" s="19">
         <v>52</v>
       </c>
-      <c r="F26" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8">
+      <c r="F26" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H26" s="27" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="29"/>
       <c r="B27" t="s">
-        <v>867</v>
-      </c>
-      <c r="C27" s="20">
+        <v>878</v>
+      </c>
+      <c r="C27" s="19">
+        <v>38</v>
+      </c>
+      <c r="F27" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H27" s="27" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="29"/>
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="19">
+        <v>22</v>
+      </c>
+      <c r="F28" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H28" s="27" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="29"/>
+      <c r="B29" t="s">
+        <v>822</v>
+      </c>
+      <c r="C29" s="19">
+        <v>20</v>
+      </c>
+      <c r="F29" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="19" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="29"/>
+      <c r="B30" t="s">
+        <v>860</v>
+      </c>
+      <c r="C30" s="19">
         <v>81</v>
       </c>
-      <c r="F27" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8">
-      <c r="B28" t="s">
-        <v>868</v>
-      </c>
-      <c r="C28" s="20">
+      <c r="F30" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="27" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="29"/>
+      <c r="B31" t="s">
+        <v>861</v>
+      </c>
+      <c r="C31" s="19">
         <v>177</v>
       </c>
-      <c r="F28" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8">
-      <c r="B29" t="s">
+      <c r="F31" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H31" s="27" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="F32" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="30" t="s">
+        <v>883</v>
+      </c>
+      <c r="B33" t="s">
+        <v>837</v>
+      </c>
+      <c r="C33" s="19">
+        <v>244</v>
+      </c>
+      <c r="F33" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="30"/>
+      <c r="B34" t="s">
+        <v>838</v>
+      </c>
+      <c r="C34" s="19">
+        <v>18</v>
+      </c>
+      <c r="F34" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="30"/>
+      <c r="B35" t="s">
+        <v>839</v>
+      </c>
+      <c r="C35" s="19">
+        <v>12</v>
+      </c>
+      <c r="F35" s="20">
+        <f t="shared" ref="F35:F66" si="1">IF(AND(D35=0,D35&lt;&gt;""),100,IF(ISERROR(E35/D35*100),0,ROUNDUP(E35/D35 * 100, 0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="30"/>
+      <c r="B36" t="s">
+        <v>840</v>
+      </c>
+      <c r="C36" s="19">
+        <v>36</v>
+      </c>
+      <c r="F36" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="30"/>
+      <c r="B37" t="s">
+        <v>841</v>
+      </c>
+      <c r="C37" s="19">
+        <v>14</v>
+      </c>
+      <c r="F37" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="30"/>
+      <c r="B38" s="21" t="s">
+        <v>836</v>
+      </c>
+      <c r="C38" s="19">
+        <v>293</v>
+      </c>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G38" s="19" t="s">
+        <v>794</v>
+      </c>
+      <c r="H38" s="19" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="30"/>
+      <c r="B39" t="s">
         <v>842</v>
       </c>
-      <c r="C29" s="20">
-        <v>244</v>
-      </c>
-      <c r="F29" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8">
-      <c r="B30" t="s">
+      <c r="C39" s="19">
+        <v>678</v>
+      </c>
+      <c r="F39" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="30"/>
+      <c r="B40" t="s">
         <v>843</v>
       </c>
-      <c r="C30" s="20">
+      <c r="C40" s="19">
+        <v>177</v>
+      </c>
+      <c r="F40" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="30"/>
+      <c r="B41" t="s">
+        <v>844</v>
+      </c>
+      <c r="C41" s="19">
+        <v>678</v>
+      </c>
+      <c r="F41" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="30"/>
+      <c r="B42" t="s">
+        <v>845</v>
+      </c>
+      <c r="C42" s="19">
+        <v>4</v>
+      </c>
+      <c r="F42" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="30"/>
+      <c r="B43" t="s">
+        <v>846</v>
+      </c>
+      <c r="C43" s="19">
+        <v>27</v>
+      </c>
+      <c r="F43" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="30"/>
+      <c r="B44" t="s">
+        <v>623</v>
+      </c>
+      <c r="C44" s="19">
+        <v>81</v>
+      </c>
+      <c r="F44" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="30"/>
+      <c r="B45" t="s">
+        <v>847</v>
+      </c>
+      <c r="C45" s="19">
+        <v>657</v>
+      </c>
+      <c r="F45" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="30"/>
+      <c r="B46" t="s">
+        <v>882</v>
+      </c>
+      <c r="C46" s="19">
+        <v>12</v>
+      </c>
+      <c r="F46" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="F47" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="30" t="s">
+        <v>884</v>
+      </c>
+      <c r="B48" t="s">
+        <v>848</v>
+      </c>
+      <c r="C48" s="19">
+        <v>53</v>
+      </c>
+      <c r="F48" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="30"/>
+      <c r="B49" t="s">
+        <v>849</v>
+      </c>
+      <c r="C49" s="19">
+        <v>52</v>
+      </c>
+      <c r="F49" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="30"/>
+      <c r="B50" t="s">
+        <v>850</v>
+      </c>
+      <c r="C50" s="19">
+        <v>7</v>
+      </c>
+      <c r="F50" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="30"/>
+      <c r="B51" t="s">
+        <v>851</v>
+      </c>
+      <c r="C51" s="19">
         <v>125</v>
       </c>
-      <c r="F30" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8">
-      <c r="B31" t="s">
-        <v>844</v>
-      </c>
-      <c r="C31" s="20">
-        <v>12</v>
-      </c>
-      <c r="F31" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8">
-      <c r="B32" t="s">
-        <v>845</v>
-      </c>
-      <c r="C32" s="20">
-        <v>36</v>
-      </c>
-      <c r="F32" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6">
-      <c r="B33" t="s">
-        <v>846</v>
-      </c>
-      <c r="C33" s="20">
-        <v>14</v>
-      </c>
-      <c r="F33" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6">
-      <c r="B34" t="s">
-        <v>847</v>
-      </c>
-      <c r="C34" s="20">
-        <v>678</v>
-      </c>
-      <c r="F34" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6">
-      <c r="B35" t="s">
-        <v>848</v>
-      </c>
-      <c r="C35" s="20">
-        <v>177</v>
-      </c>
-      <c r="F35" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6">
-      <c r="B36" t="s">
-        <v>849</v>
-      </c>
-      <c r="C36" s="20">
-        <v>678</v>
-      </c>
-      <c r="F36" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6">
-      <c r="B37" t="s">
-        <v>850</v>
-      </c>
-      <c r="C37" s="20">
-        <v>4</v>
-      </c>
-      <c r="F37" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6">
-      <c r="B38" t="s">
-        <v>851</v>
-      </c>
-      <c r="C38" s="20">
-        <v>27</v>
-      </c>
-      <c r="F38" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6">
-      <c r="B39" t="s">
-        <v>623</v>
-      </c>
-      <c r="C39" s="20">
-        <v>81</v>
-      </c>
-      <c r="F39" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6">
-      <c r="B40" t="s">
+      <c r="F51" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="30"/>
+      <c r="B52" t="s">
         <v>852</v>
       </c>
-      <c r="C40" s="20">
-        <v>657</v>
-      </c>
-      <c r="F40" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6">
-      <c r="B41" t="s">
+      <c r="C52" s="19">
+        <v>183</v>
+      </c>
+      <c r="F52" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="30"/>
+      <c r="B53" t="s">
         <v>853</v>
       </c>
-      <c r="C41" s="20">
-        <v>53</v>
-      </c>
-      <c r="F41" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6">
-      <c r="B42" t="s">
+      <c r="C53" s="19">
+        <v>34</v>
+      </c>
+      <c r="F53" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="30"/>
+      <c r="B54" t="s">
         <v>854</v>
       </c>
-      <c r="C42" s="20">
-        <v>52</v>
-      </c>
-      <c r="F42" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6">
-      <c r="B43" t="s">
+      <c r="C54" s="19">
+        <v>114</v>
+      </c>
+      <c r="F54" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="30"/>
+      <c r="B55" t="s">
         <v>855</v>
       </c>
-      <c r="C43" s="20">
-        <v>7</v>
-      </c>
-      <c r="F43" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6">
-      <c r="B44" t="s">
-        <v>856</v>
-      </c>
-      <c r="C44" s="20">
-        <v>125</v>
-      </c>
-      <c r="F44" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6">
-      <c r="B45" t="s">
-        <v>857</v>
-      </c>
-      <c r="C45" s="20">
-        <v>183</v>
-      </c>
-      <c r="F45" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6">
-      <c r="B46" t="s">
-        <v>858</v>
-      </c>
-      <c r="C46" s="20">
-        <v>34</v>
-      </c>
-      <c r="F46" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6">
-      <c r="B47" t="s">
-        <v>859</v>
-      </c>
-      <c r="C47" s="20">
-        <v>114</v>
-      </c>
-      <c r="F47" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6">
-      <c r="B48" t="s">
-        <v>860</v>
-      </c>
-      <c r="C48" s="20">
+      <c r="C55" s="19">
         <v>28</v>
       </c>
-      <c r="F48" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8">
-      <c r="B49" t="s">
+      <c r="F55" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="30"/>
+      <c r="B56" t="s">
         <v>747</v>
       </c>
-      <c r="C49" s="20">
+      <c r="C56" s="19">
         <v>738</v>
       </c>
-      <c r="F49" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="50" spans="2:8">
-      <c r="B50" t="s">
-        <v>870</v>
-      </c>
-      <c r="C50" s="20">
-        <v>2</v>
-      </c>
-      <c r="D50" s="20">
-        <v>2</v>
-      </c>
-      <c r="E50" s="20">
-        <v>2</v>
-      </c>
-      <c r="F50" t="s">
-        <v>832</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8">
-      <c r="B51" t="s">
-        <v>871</v>
-      </c>
-      <c r="C51" s="20">
-        <v>1</v>
-      </c>
-      <c r="D51" s="20">
+      <c r="F56" s="20">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E51" s="20">
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="19"/>
+      <c r="F57" s="26">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F51" t="s">
-        <v>832</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8">
-      <c r="B52" s="23" t="s">
-        <v>869</v>
-      </c>
-      <c r="C52" s="24">
-        <f>SUM(Table13[Total Cases])</f>
-        <v>5205</v>
-      </c>
-      <c r="D52" s="24">
-        <f>SUM(Table13[Automation Candidates])</f>
+    </row>
+    <row r="58" spans="1:8" ht="15" thickBot="1">
+      <c r="A58" s="19" t="s">
+        <v>885</v>
+      </c>
+      <c r="C58" s="19">
+        <v>1929</v>
+      </c>
+      <c r="F58" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="15" thickTop="1">
+      <c r="B59" s="22" t="s">
+        <v>862</v>
+      </c>
+      <c r="C59" s="23">
+        <f>SUM(Table13[Total Test Case '#])</f>
+        <v>7099</v>
+      </c>
+      <c r="D59" s="23">
+        <f>SUM(Table13[Automation Candidate '#])</f>
         <v>420</v>
       </c>
-      <c r="E52" s="24">
-        <f>SUM(Table13[Complete Cases])</f>
-        <v>279</v>
-      </c>
-      <c r="F52" s="23"/>
-      <c r="G52" s="24"/>
-      <c r="H52" s="23"/>
+      <c r="E59" s="23">
+        <f>SUM(Table13[Automated Case '#])</f>
+        <v>265</v>
+      </c>
+      <c r="F59" s="24">
+        <f>ROUNDUP(E59/D59 * 100, 0)</f>
+        <v>64</v>
+      </c>
+      <c r="G59" s="23"/>
+      <c r="H59" s="28"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A3:A31"/>
+    <mergeCell ref="A33:A46"/>
+    <mergeCell ref="A48:A56"/>
+  </mergeCells>
+  <conditionalFormatting sqref="F3:F58">
+    <cfRule type="dataBar" priority="17">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D5103404-440E-8D44-9101-0B9FCCB94B01}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F58">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F58">
+    <cfRule type="dataBar" priority="19">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{075DC176-F228-8345-995E-BE9BC87D8BCF}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D5103404-440E-8D44-9101-0B9FCCB94B01}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F3:F58</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{075DC176-F228-8345-995E-BE9BC87D8BCF}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F3:F58</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>

</xml_diff>

<commit_message>
1. Bump incompleted phase I clean up task into Phase II. 2. Reorder feature.
Change-Id: I6e42c751f32dff3911d1a57974caa9c280068930
Reviewed-on: https://gerrit.dechocorp.com/47484
Reviewed-by: James Cookson <jcookson@vmware.com>
Reviewed-by: Spark Yao <shipuy@mozy.com>
</commit_message>
<xml_diff>
--- a/automation_tracking.xlsx
+++ b/automation_tracking.xlsx
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4192" uniqueCount="886">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4244" uniqueCount="894">
   <si>
     <t>Billing Automation Test Plan</t>
   </si>
@@ -2738,19 +2738,43 @@
     <t>Cleaning up cases</t>
   </si>
   <si>
-    <t>Phase I</t>
-  </si>
-  <si>
     <t>Smoke Test (for production)</t>
   </si>
   <si>
-    <t>Phase II</t>
-  </si>
-  <si>
-    <t>Phase III</t>
-  </si>
-  <si>
-    <t>Phase IV</t>
+    <t>Cleanup Owner</t>
+  </si>
+  <si>
+    <t>Dave</t>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>Rob</t>
+  </si>
+  <si>
+    <t>Neale</t>
+  </si>
+  <si>
+    <t>Rob and Neale</t>
+  </si>
+  <si>
+    <t>Catherine</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t>IV</t>
   </si>
 </sst>
 </file>
@@ -2760,7 +2784,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-409]mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm;@"/>
-    <numFmt numFmtId="168" formatCode="00000"/>
+    <numFmt numFmtId="166" formatCode="00000"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -2861,7 +2885,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2925,8 +2949,32 @@
         <bgColor theme="4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -2984,8 +3032,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="118">
+  <cellStyleXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -3104,8 +3163,24 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
@@ -3143,9 +3218,6 @@
     <xf numFmtId="0" fontId="13" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3155,14 +3227,36 @@
     <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="118">
+  <cellStyles count="134">
     <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
     <cellStyle name="20% - Accent2" xfId="5" builtinId="34"/>
     <cellStyle name="20% - Accent3" xfId="6" builtinId="38"/>
@@ -3223,6 +3317,14 @@
     <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
@@ -3278,11 +3380,19 @@
     <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="16">
     <dxf>
       <font>
         <b/>
@@ -3340,6 +3450,42 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color theme="0"/>
@@ -3531,10 +3677,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3544,6 +3686,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
@@ -3551,6 +3697,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -3583,23 +3732,24 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B2:H59" totalsRowCount="1" headerRowDxfId="8">
-  <autoFilter ref="B2:H58"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="Feature Name" totalsRowLabel="Total" totalsRowDxfId="6"/>
-    <tableColumn id="2" name="Total Test Case #" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B2:I59" totalsRowCount="1" headerRowDxfId="15">
+  <autoFilter ref="B2:I58"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Feature Name" totalsRowLabel="Total" totalsRowDxfId="7"/>
+    <tableColumn id="2" name="Total Test Case #" totalsRowFunction="custom" dataDxfId="14" totalsRowDxfId="6">
       <totalsRowFormula>SUM(Table13[Total Test Case '#])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="Automation Candidate #" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="4">
+    <tableColumn id="6" name="Automation Candidate #" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="5">
       <totalsRowFormula>SUM(Table13[Automation Candidate '#])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" name="Automated Case #" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="3">
+    <tableColumn id="10" name="Automated Case #" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="4">
       <totalsRowFormula>SUM(Table13[Automated Case '#])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" name="Completion %" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="2">
+    <tableColumn id="3" name="Completion %" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="3">
       <calculatedColumnFormula>IF(AND(D3=0,D3&lt;&gt;""),100,IF(ISERROR(E3/D3*100),0,ROUNDUP(E3/D3 * 100, 0)))</calculatedColumnFormula>
       <totalsRowFormula>ROUNDUP(E59/D59 * 100, 0)</totalsRowFormula>
     </tableColumn>
+    <tableColumn id="4" name="Cleanup Owner" dataDxfId="8" totalsRowDxfId="2"/>
     <tableColumn id="7" name="Automation Owner" dataDxfId="10" totalsRowDxfId="1"/>
     <tableColumn id="11" name="Note" dataDxfId="9" totalsRowDxfId="0"/>
   </tableColumns>
@@ -20754,19 +20904,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:19">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="29" t="s">
         <v>685</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
       <c r="L2" t="s">
         <v>686</v>
       </c>
@@ -22036,25 +22186,30 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H59"/>
+  <dimension ref="A2:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" style="19" customWidth="1"/>
     <col min="4" max="5" width="11.1640625" style="19" customWidth="1"/>
     <col min="6" max="6" width="15.83203125" style="19" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.83203125" style="27" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" style="28" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.83203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="28">
+    <row r="2" spans="1:9" ht="29" thickBot="1">
+      <c r="A2" s="30" t="s">
+        <v>889</v>
+      </c>
       <c r="B2" s="20" t="s">
         <v>830</v>
       </c>
@@ -22071,15 +22226,18 @@
         <v>869</v>
       </c>
       <c r="G2" s="20" t="s">
+        <v>882</v>
+      </c>
+      <c r="H2" s="20" t="s">
         <v>876</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="I2" s="20" t="s">
         <v>828</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="29" t="s">
-        <v>881</v>
+    <row r="3" spans="1:9" ht="15" thickTop="1">
+      <c r="A3" s="32" t="s">
+        <v>890</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>831</v>
@@ -22094,18 +22252,21 @@
         <v>37</v>
       </c>
       <c r="F3" s="20">
-        <f t="shared" ref="F3:F34" si="0">IF(AND(D3=0,D3&lt;&gt;""),100,IF(ISERROR(E3/D3*100),0,ROUNDUP(E3/D3 * 100, 0)))</f>
+        <f t="shared" ref="F3:F28" si="0">IF(AND(D3=0,D3&lt;&gt;""),100,IF(ISERROR(E3/D3*100),0,ROUNDUP(E3/D3 * 100, 0)))</f>
         <v>100</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="20" t="s">
+        <v>870</v>
+      </c>
+      <c r="H3" s="19" t="s">
         <v>794</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="I3" s="19" t="s">
         <v>871</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="29"/>
+    <row r="4" spans="1:9">
+      <c r="A4" s="32"/>
       <c r="B4" s="21" t="s">
         <v>16</v>
       </c>
@@ -22122,15 +22283,18 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="20" t="s">
+        <v>870</v>
+      </c>
+      <c r="H4" s="19" t="s">
         <v>794</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="I4" s="19" t="s">
         <v>871</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="29"/>
+    <row r="5" spans="1:9">
+      <c r="A5" s="32"/>
       <c r="B5" s="21" t="s">
         <v>687</v>
       </c>
@@ -22147,15 +22311,18 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="20" t="s">
+        <v>870</v>
+      </c>
+      <c r="H5" s="19" t="s">
         <v>794</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="I5" s="19" t="s">
         <v>871</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="29"/>
+    <row r="6" spans="1:9">
+      <c r="A6" s="32"/>
       <c r="B6" s="21" t="s">
         <v>832</v>
       </c>
@@ -22172,15 +22339,18 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="20" t="s">
+        <v>870</v>
+      </c>
+      <c r="H6" s="19" t="s">
         <v>794</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="I6" s="19" t="s">
         <v>871</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="29"/>
+    <row r="7" spans="1:9">
+      <c r="A7" s="32"/>
       <c r="B7" s="21" t="s">
         <v>833</v>
       </c>
@@ -22197,15 +22367,18 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="20" t="s">
+        <v>870</v>
+      </c>
+      <c r="H7" s="19" t="s">
         <v>794</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="I7" s="19" t="s">
         <v>871</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="29"/>
+    <row r="8" spans="1:9">
+      <c r="A8" s="32"/>
       <c r="B8" s="21" t="s">
         <v>834</v>
       </c>
@@ -22222,15 +22395,18 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="20" t="s">
+        <v>870</v>
+      </c>
+      <c r="H8" s="19" t="s">
         <v>794</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="I8" s="19" t="s">
         <v>871</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="29"/>
+    <row r="9" spans="1:9">
+      <c r="A9" s="32"/>
       <c r="B9" s="21" t="s">
         <v>835</v>
       </c>
@@ -22247,15 +22423,18 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="20" t="s">
+        <v>870</v>
+      </c>
+      <c r="H9" s="19" t="s">
         <v>794</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="I9" s="19" t="s">
         <v>871</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="29"/>
+    <row r="10" spans="1:9">
+      <c r="A10" s="32"/>
       <c r="B10" s="21" t="s">
         <v>856</v>
       </c>
@@ -22272,15 +22451,18 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="20" t="s">
+        <v>870</v>
+      </c>
+      <c r="H10" s="19" t="s">
         <v>794</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="I10" s="19" t="s">
         <v>871</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="29"/>
+    <row r="11" spans="1:9">
+      <c r="A11" s="32"/>
       <c r="B11" s="21" t="s">
         <v>857</v>
       </c>
@@ -22297,15 +22479,18 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="20" t="s">
+        <v>870</v>
+      </c>
+      <c r="H11" s="19" t="s">
         <v>794</v>
       </c>
-      <c r="H11" s="19" t="s">
+      <c r="I11" s="19" t="s">
         <v>871</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="29"/>
+    <row r="12" spans="1:9">
+      <c r="A12" s="32"/>
       <c r="B12" s="21" t="s">
         <v>858</v>
       </c>
@@ -22322,15 +22507,18 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="20" t="s">
+        <v>870</v>
+      </c>
+      <c r="H12" s="19" t="s">
         <v>796</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="I12" s="19" t="s">
         <v>871</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="29"/>
+    <row r="13" spans="1:9">
+      <c r="A13" s="32"/>
       <c r="B13" s="21" t="s">
         <v>859</v>
       </c>
@@ -22347,15 +22535,18 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="G13" s="20" t="s">
+        <v>870</v>
+      </c>
+      <c r="H13" s="19" t="s">
         <v>796</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="I13" s="19" t="s">
         <v>871</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="29"/>
+    <row r="14" spans="1:9">
+      <c r="A14" s="32"/>
       <c r="B14" t="s">
         <v>817</v>
       </c>
@@ -22372,15 +22563,18 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="20" t="s">
+        <v>870</v>
+      </c>
+      <c r="H14" s="19" t="s">
         <v>794</v>
       </c>
-      <c r="H14" s="19" t="s">
+      <c r="I14" s="19" t="s">
         <v>871</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="29"/>
+    <row r="15" spans="1:9">
+      <c r="A15" s="32"/>
       <c r="B15" t="s">
         <v>821</v>
       </c>
@@ -22397,15 +22591,18 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="G15" s="20" t="s">
         <v>870</v>
       </c>
       <c r="H15" s="19" t="s">
+        <v>870</v>
+      </c>
+      <c r="I15" s="19" t="s">
         <v>871</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="29"/>
+    <row r="16" spans="1:9">
+      <c r="A16" s="32"/>
       <c r="B16" t="s">
         <v>819</v>
       </c>
@@ -22422,15 +22619,18 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G16" s="19" t="s">
+      <c r="G16" s="20" t="s">
         <v>870</v>
       </c>
       <c r="H16" s="19" t="s">
+        <v>870</v>
+      </c>
+      <c r="I16" s="19" t="s">
         <v>871</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="29"/>
+    <row r="17" spans="1:9">
+      <c r="A17" s="32"/>
       <c r="B17" t="s">
         <v>863</v>
       </c>
@@ -22447,15 +22647,18 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="G17" s="20" t="s">
+        <v>870</v>
+      </c>
+      <c r="H17" s="19" t="s">
         <v>796</v>
       </c>
-      <c r="H17" s="27" t="s">
+      <c r="I17" s="26" t="s">
         <v>871</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="29"/>
+    <row r="18" spans="1:9">
+      <c r="A18" s="32"/>
       <c r="B18" t="s">
         <v>864</v>
       </c>
@@ -22472,15 +22675,18 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="G18" s="20" t="s">
         <v>870</v>
       </c>
-      <c r="H18" s="27" t="s">
+      <c r="H18" s="19" t="s">
+        <v>870</v>
+      </c>
+      <c r="I18" s="26" t="s">
         <v>871</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="29"/>
+    <row r="19" spans="1:9">
+      <c r="A19" s="32"/>
       <c r="B19" t="s">
         <v>818</v>
       </c>
@@ -22497,15 +22703,18 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="G19" s="19" t="s">
+      <c r="G19" s="20" t="s">
+        <v>883</v>
+      </c>
+      <c r="H19" s="19" t="s">
         <v>794</v>
       </c>
-      <c r="H19" s="27" t="s">
+      <c r="I19" s="26" t="s">
         <v>873</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="29"/>
+    <row r="20" spans="1:9">
+      <c r="A20" s="32"/>
       <c r="B20" t="s">
         <v>820</v>
       </c>
@@ -22522,15 +22731,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G20" s="19" t="s">
+      <c r="G20" s="20" t="s">
         <v>829</v>
       </c>
-      <c r="H20" s="27" t="s">
+      <c r="H20" s="19" t="s">
+        <v>829</v>
+      </c>
+      <c r="I20" s="26" t="s">
         <v>873</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="29"/>
+    <row r="21" spans="1:9">
+      <c r="A21" s="32"/>
       <c r="B21" t="s">
         <v>865</v>
       </c>
@@ -22547,15 +22759,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G21" s="19" t="s">
+      <c r="G21" s="20" t="s">
+        <v>883</v>
+      </c>
+      <c r="H21" s="19" t="s">
         <v>829</v>
       </c>
-      <c r="H21" s="27" t="s">
+      <c r="I21" s="26" t="s">
         <v>873</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="29"/>
+    <row r="22" spans="1:9">
+      <c r="A22" s="32"/>
       <c r="B22" t="s">
         <v>825</v>
       </c>
@@ -22572,15 +22787,18 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G22" s="19" t="s">
+      <c r="G22" s="20" t="s">
+        <v>883</v>
+      </c>
+      <c r="H22" s="19" t="s">
         <v>866</v>
       </c>
-      <c r="H22" s="27" t="s">
+      <c r="I22" s="26" t="s">
         <v>873</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="29"/>
+    <row r="23" spans="1:9">
+      <c r="A23" s="32"/>
       <c r="B23" t="s">
         <v>826</v>
       </c>
@@ -22597,15 +22815,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" s="19" t="s">
+      <c r="G23" s="20" t="s">
+        <v>883</v>
+      </c>
+      <c r="H23" s="19" t="s">
         <v>866</v>
       </c>
-      <c r="H23" s="27" t="s">
+      <c r="I23" s="26" t="s">
         <v>873</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="29"/>
+    <row r="24" spans="1:9">
+      <c r="A24" s="32"/>
       <c r="B24" t="s">
         <v>827</v>
       </c>
@@ -22622,15 +22843,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G24" s="19" t="s">
+      <c r="G24" s="20" t="s">
+        <v>884</v>
+      </c>
+      <c r="H24" s="19" t="s">
         <v>829</v>
       </c>
-      <c r="H24" s="27" t="s">
+      <c r="I24" s="26" t="s">
         <v>873</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="29"/>
+    <row r="25" spans="1:9">
+      <c r="A25" s="32"/>
       <c r="B25" t="s">
         <v>823</v>
       </c>
@@ -22647,313 +22871,405 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H25" s="27" t="s">
+      <c r="G25" s="20" t="s">
+        <v>829</v>
+      </c>
+      <c r="H25" s="19" t="s">
+        <v>829</v>
+      </c>
+      <c r="I25" s="26" t="s">
         <v>874</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="29"/>
-      <c r="B26" t="s">
-        <v>824</v>
-      </c>
-      <c r="C26" s="19">
-        <v>52</v>
-      </c>
-      <c r="F26" s="20">
+    <row r="26" spans="1:9">
+      <c r="B26" s="34"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="27" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="29"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="37"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="31" t="s">
+        <v>891</v>
+      </c>
       <c r="B27" t="s">
-        <v>878</v>
+        <v>837</v>
       </c>
       <c r="C27" s="19">
-        <v>38</v>
-      </c>
-      <c r="F27" s="26">
+        <v>244</v>
+      </c>
+      <c r="F27" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H27" s="27" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="29"/>
+      <c r="G27" s="20" t="s">
+        <v>829</v>
+      </c>
+      <c r="H27" s="19" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="31"/>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>838</v>
       </c>
       <c r="C28" s="19">
-        <v>22</v>
-      </c>
-      <c r="F28" s="26">
+        <v>18</v>
+      </c>
+      <c r="F28" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H28" s="27" t="s">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="29"/>
+      <c r="G28" s="20" t="s">
+        <v>829</v>
+      </c>
+      <c r="H28" s="19" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="31"/>
       <c r="B29" t="s">
-        <v>822</v>
+        <v>840</v>
       </c>
       <c r="C29" s="19">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="F29" s="20">
-        <f t="shared" si="0"/>
+        <f>IF(AND(D29=0,D29&lt;&gt;""),100,IF(ISERROR(E29/D29*100),0,ROUNDUP(E29/D29 * 100, 0)))</f>
         <v>0</v>
       </c>
+      <c r="G29" s="20" t="s">
+        <v>829</v>
+      </c>
       <c r="H29" s="19" t="s">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="29"/>
-      <c r="B30" t="s">
-        <v>860</v>
+        <v>829</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="31"/>
+      <c r="B30" s="21" t="s">
+        <v>836</v>
       </c>
       <c r="C30" s="19">
-        <v>81</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
       <c r="F30" s="20">
-        <f t="shared" si="0"/>
+        <f>IF(AND(D30=0,D30&lt;&gt;""),100,IF(ISERROR(E30/D30*100),0,ROUNDUP(E30/D30 * 100, 0)))</f>
         <v>0</v>
       </c>
-      <c r="H30" s="27" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="29"/>
+      <c r="G30" s="20" t="s">
+        <v>794</v>
+      </c>
+      <c r="H30" s="19" t="s">
+        <v>794</v>
+      </c>
+      <c r="I30" s="19" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="31"/>
       <c r="B31" t="s">
-        <v>861</v>
+        <v>843</v>
       </c>
       <c r="C31" s="19">
         <v>177</v>
       </c>
       <c r="F31" s="20">
-        <f t="shared" si="0"/>
+        <f>IF(AND(D31=0,D31&lt;&gt;""),100,IF(ISERROR(E31/D31*100),0,ROUNDUP(E31/D31 * 100, 0)))</f>
         <v>0</v>
       </c>
-      <c r="H31" s="27" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="F32" s="26">
-        <f t="shared" si="0"/>
+      <c r="G31" s="20" t="s">
+        <v>829</v>
+      </c>
+      <c r="H31" s="19" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="31"/>
+      <c r="B32" t="s">
+        <v>839</v>
+      </c>
+      <c r="C32" s="19">
+        <v>12</v>
+      </c>
+      <c r="F32" s="20">
+        <f t="shared" ref="F32:F58" si="1">IF(AND(D32=0,D32&lt;&gt;""),100,IF(ISERROR(E32/D32*100),0,ROUNDUP(E32/D32 * 100, 0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="30" t="s">
-        <v>883</v>
-      </c>
+      <c r="G32" s="20" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="31"/>
       <c r="B33" t="s">
-        <v>837</v>
+        <v>841</v>
       </c>
       <c r="C33" s="19">
-        <v>244</v>
+        <v>14</v>
       </c>
       <c r="F33" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="30"/>
+      <c r="G33" s="20" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="28">
+      <c r="A34" s="31"/>
       <c r="B34" t="s">
-        <v>838</v>
+        <v>842</v>
       </c>
       <c r="C34" s="19">
-        <v>18</v>
+        <v>678</v>
       </c>
       <c r="F34" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="30"/>
+      <c r="G34" s="20" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="28">
+      <c r="A35" s="31"/>
       <c r="B35" t="s">
-        <v>839</v>
+        <v>844</v>
       </c>
       <c r="C35" s="19">
-        <v>12</v>
+        <v>678</v>
       </c>
       <c r="F35" s="20">
-        <f t="shared" ref="F35:F66" si="1">IF(AND(D35=0,D35&lt;&gt;""),100,IF(ISERROR(E35/D35*100),0,ROUNDUP(E35/D35 * 100, 0)))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="30"/>
+      <c r="G35" s="20" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="31"/>
       <c r="B36" t="s">
-        <v>840</v>
+        <v>845</v>
       </c>
       <c r="C36" s="19">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="F36" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="30"/>
+      <c r="G36" s="20" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="31"/>
       <c r="B37" t="s">
-        <v>841</v>
+        <v>846</v>
       </c>
       <c r="C37" s="19">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="F37" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="30"/>
-      <c r="B38" s="21" t="s">
-        <v>836</v>
+      <c r="G37" s="20" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="31"/>
+      <c r="B38" t="s">
+        <v>623</v>
       </c>
       <c r="C38" s="19">
-        <v>293</v>
-      </c>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
+        <v>81</v>
+      </c>
       <c r="F38" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G38" s="19" t="s">
-        <v>794</v>
-      </c>
-      <c r="H38" s="19" t="s">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="30"/>
+      <c r="G38" s="20" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="28">
+      <c r="A39" s="31"/>
       <c r="B39" t="s">
-        <v>842</v>
+        <v>847</v>
       </c>
       <c r="C39" s="19">
-        <v>678</v>
+        <v>657</v>
       </c>
       <c r="F39" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="30"/>
+      <c r="G39" s="20" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="31"/>
       <c r="B40" t="s">
-        <v>843</v>
+        <v>881</v>
       </c>
       <c r="C40" s="19">
-        <v>177</v>
-      </c>
-      <c r="F40" s="20">
+        <v>12</v>
+      </c>
+      <c r="F40" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="30"/>
+      <c r="G40" s="25" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="31"/>
       <c r="B41" t="s">
-        <v>844</v>
+        <v>824</v>
       </c>
       <c r="C41" s="19">
-        <v>678</v>
+        <v>52</v>
       </c>
       <c r="F41" s="20">
+        <f>IF(AND(D41=0,D41&lt;&gt;""),100,IF(ISERROR(E41/D41*100),0,ROUNDUP(E41/D41 * 100, 0)))</f>
+        <v>0</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>885</v>
+      </c>
+      <c r="I41" s="26" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="31"/>
+      <c r="B42" t="s">
+        <v>878</v>
+      </c>
+      <c r="C42" s="19">
+        <v>38</v>
+      </c>
+      <c r="F42" s="25">
+        <f>IF(AND(D42=0,D42&lt;&gt;""),100,IF(ISERROR(E42/D42*100),0,ROUNDUP(E42/D42 * 100, 0)))</f>
+        <v>0</v>
+      </c>
+      <c r="G42" s="25" t="s">
+        <v>885</v>
+      </c>
+      <c r="I42" s="26" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="31"/>
+      <c r="B43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="19">
+        <v>22</v>
+      </c>
+      <c r="F43" s="25">
+        <f>IF(AND(D43=0,D43&lt;&gt;""),100,IF(ISERROR(E43/D43*100),0,ROUNDUP(E43/D43 * 100, 0)))</f>
+        <v>0</v>
+      </c>
+      <c r="G43" s="25" t="s">
+        <v>886</v>
+      </c>
+      <c r="I43" s="26" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="31"/>
+      <c r="B44" t="s">
+        <v>822</v>
+      </c>
+      <c r="C44" s="19">
+        <v>20</v>
+      </c>
+      <c r="F44" s="20">
+        <f>IF(AND(D44=0,D44&lt;&gt;""),100,IF(ISERROR(E44/D44*100),0,ROUNDUP(E44/D44 * 100, 0)))</f>
+        <v>0</v>
+      </c>
+      <c r="G44" s="20" t="s">
+        <v>886</v>
+      </c>
+      <c r="I44" s="19" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="31"/>
+      <c r="B45" t="s">
+        <v>860</v>
+      </c>
+      <c r="C45" s="19">
+        <v>81</v>
+      </c>
+      <c r="F45" s="20">
+        <f>IF(AND(D45=0,D45&lt;&gt;""),100,IF(ISERROR(E45/D45*100),0,ROUNDUP(E45/D45 * 100, 0)))</f>
+        <v>0</v>
+      </c>
+      <c r="G45" s="20" t="s">
+        <v>877</v>
+      </c>
+      <c r="I45" s="26" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="31"/>
+      <c r="B46" t="s">
+        <v>861</v>
+      </c>
+      <c r="C46" s="19">
+        <v>177</v>
+      </c>
+      <c r="F46" s="20">
+        <f>IF(AND(D46=0,D46&lt;&gt;""),100,IF(ISERROR(E46/D46*100),0,ROUNDUP(E46/D46 * 100, 0)))</f>
+        <v>0</v>
+      </c>
+      <c r="G46" s="20" t="s">
+        <v>877</v>
+      </c>
+      <c r="I46" s="26" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="B47" s="34"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="35"/>
+      <c r="F47" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="30"/>
-      <c r="B42" t="s">
-        <v>845</v>
-      </c>
-      <c r="C42" s="19">
-        <v>4</v>
-      </c>
-      <c r="F42" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="30"/>
-      <c r="B43" t="s">
-        <v>846</v>
-      </c>
-      <c r="C43" s="19">
-        <v>27</v>
-      </c>
-      <c r="F43" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="30"/>
-      <c r="B44" t="s">
-        <v>623</v>
-      </c>
-      <c r="C44" s="19">
-        <v>81</v>
-      </c>
-      <c r="F44" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="30"/>
-      <c r="B45" t="s">
-        <v>847</v>
-      </c>
-      <c r="C45" s="19">
-        <v>657</v>
-      </c>
-      <c r="F45" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="30"/>
-      <c r="B46" t="s">
-        <v>882</v>
-      </c>
-      <c r="C46" s="19">
-        <v>12</v>
-      </c>
-      <c r="F46" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="F47" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="30" t="s">
-        <v>884</v>
+      <c r="G47" s="36"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="37"/>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="33" t="s">
+        <v>892</v>
       </c>
       <c r="B48" t="s">
         <v>848</v>
@@ -22965,9 +23281,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="30"/>
+      <c r="G48" s="20" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="33"/>
       <c r="B49" t="s">
         <v>849</v>
       </c>
@@ -22978,9 +23297,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:8">
-      <c r="A50" s="30"/>
+      <c r="G49" s="20" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="33"/>
       <c r="B50" t="s">
         <v>850</v>
       </c>
@@ -22991,9 +23313,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="30"/>
+      <c r="G50" s="20"/>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="33"/>
       <c r="B51" t="s">
         <v>851</v>
       </c>
@@ -23004,9 +23327,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="30"/>
+      <c r="G51" s="20"/>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="33"/>
       <c r="B52" t="s">
         <v>852</v>
       </c>
@@ -23017,9 +23341,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:8">
-      <c r="A53" s="30"/>
+      <c r="G52" s="20"/>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="33"/>
       <c r="B53" t="s">
         <v>853</v>
       </c>
@@ -23030,9 +23355,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54" s="30"/>
+      <c r="G53" s="20"/>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="33"/>
       <c r="B54" t="s">
         <v>854</v>
       </c>
@@ -23043,9 +23369,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:8">
-      <c r="A55" s="30"/>
+      <c r="G54" s="20"/>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="33"/>
       <c r="B55" t="s">
         <v>855</v>
       </c>
@@ -23056,9 +23383,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:8">
-      <c r="A56" s="30"/>
+      <c r="G55" s="20"/>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="33"/>
       <c r="B56" t="s">
         <v>747</v>
       </c>
@@ -23069,27 +23397,36 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:8">
+      <c r="G56" s="20"/>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57" s="19"/>
-      <c r="F57" s="26">
+      <c r="B57" s="34"/>
+      <c r="C57" s="35"/>
+      <c r="D57" s="35"/>
+      <c r="E57" s="35"/>
+      <c r="F57" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" ht="15" thickBot="1">
+      <c r="G57" s="36"/>
+      <c r="H57" s="35"/>
+      <c r="I57" s="37"/>
+    </row>
+    <row r="58" spans="1:9" ht="15" thickBot="1">
       <c r="A58" s="19" t="s">
-        <v>885</v>
+        <v>893</v>
       </c>
       <c r="C58" s="19">
         <v>1929</v>
       </c>
-      <c r="F58" s="26">
+      <c r="F58" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" ht="15" thickTop="1">
+      <c r="G58" s="25"/>
+    </row>
+    <row r="59" spans="1:9" ht="15" thickTop="1">
       <c r="B59" s="22" t="s">
         <v>862</v>
       </c>
@@ -23109,16 +23446,17 @@
         <f>ROUNDUP(E59/D59 * 100, 0)</f>
         <v>64</v>
       </c>
-      <c r="G59" s="23"/>
-      <c r="H59" s="28"/>
+      <c r="G59" s="24"/>
+      <c r="H59" s="23"/>
+      <c r="I59" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A3:A31"/>
-    <mergeCell ref="A33:A46"/>
     <mergeCell ref="A48:A56"/>
+    <mergeCell ref="A3:A25"/>
+    <mergeCell ref="A27:A46"/>
   </mergeCells>
-  <conditionalFormatting sqref="F3:F58">
+  <conditionalFormatting sqref="F3:G58">
     <cfRule type="dataBar" priority="17">
       <dataBar>
         <cfvo type="min"/>
@@ -23132,7 +23470,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F58">
+  <conditionalFormatting sqref="F3:G58">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -23144,7 +23482,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F58">
+  <conditionalFormatting sqref="F3:G58">
     <cfRule type="dataBar" priority="19">
       <dataBar>
         <cfvo type="min"/>
@@ -23177,7 +23515,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F3:F58</xm:sqref>
+          <xm:sqref>F3:G58</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{075DC176-F228-8345-995E-BE9BC87D8BCF}">
@@ -23190,7 +23528,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F3:F58</xm:sqref>
+          <xm:sqref>F3:G58</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Add test cases for bus/regression/admins TC.695 ~ TC.700 6 cases. Test in QA6 busclient01, 2.4.0.17
Change-Id: I7ad6aced35e74b1a9148727e23fc6ce1aff8071a
Reviewed-on: https://gerrit.dechocorp.com/47962
Reviewed-by: Spark Yao <shipuy@mozy.com>
</commit_message>
<xml_diff>
--- a/automation_tracking.xlsx
+++ b/automation_tracking.xlsx
@@ -3230,20 +3230,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3254,6 +3242,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="134">
@@ -3677,13 +3677,13 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -3749,9 +3749,9 @@
       <calculatedColumnFormula>IF(AND(D3=0,D3&lt;&gt;""),100,IF(ISERROR(E3/D3*100),0,ROUNDUP(E3/D3 * 100, 0)))</calculatedColumnFormula>
       <totalsRowFormula>ROUNDUP(E59/D59 * 100, 0)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" name="Cleanup Owner" dataDxfId="8" totalsRowDxfId="2"/>
-    <tableColumn id="7" name="Automation Owner" dataDxfId="10" totalsRowDxfId="1"/>
-    <tableColumn id="11" name="Note" dataDxfId="9" totalsRowDxfId="0"/>
+    <tableColumn id="4" name="Cleanup Owner" dataDxfId="10" totalsRowDxfId="2"/>
+    <tableColumn id="7" name="Automation Owner" dataDxfId="9" totalsRowDxfId="1"/>
+    <tableColumn id="11" name="Note" dataDxfId="8" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -20904,19 +20904,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:19">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="34" t="s">
         <v>685</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
       <c r="L2" t="s">
         <v>686</v>
       </c>
@@ -22188,8 +22188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -22207,7 +22207,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="29" thickBot="1">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="29" t="s">
         <v>889</v>
       </c>
       <c r="B2" s="20" t="s">
@@ -22236,7 +22236,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15" thickTop="1">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="36" t="s">
         <v>890</v>
       </c>
       <c r="B3" s="21" t="s">
@@ -22266,7 +22266,7 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="32"/>
+      <c r="A4" s="36"/>
       <c r="B4" s="21" t="s">
         <v>16</v>
       </c>
@@ -22294,7 +22294,7 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="32"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="21" t="s">
         <v>687</v>
       </c>
@@ -22322,7 +22322,7 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="32"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="21" t="s">
         <v>832</v>
       </c>
@@ -22350,7 +22350,7 @@
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="32"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="21" t="s">
         <v>833</v>
       </c>
@@ -22378,7 +22378,7 @@
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="32"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="21" t="s">
         <v>834</v>
       </c>
@@ -22406,7 +22406,7 @@
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="32"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="21" t="s">
         <v>835</v>
       </c>
@@ -22434,7 +22434,7 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="32"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="21" t="s">
         <v>856</v>
       </c>
@@ -22462,7 +22462,7 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="32"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="21" t="s">
         <v>857</v>
       </c>
@@ -22490,7 +22490,7 @@
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="32"/>
+      <c r="A12" s="36"/>
       <c r="B12" s="21" t="s">
         <v>858</v>
       </c>
@@ -22518,7 +22518,7 @@
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="32"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="21" t="s">
         <v>859</v>
       </c>
@@ -22546,7 +22546,7 @@
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="32"/>
+      <c r="A14" s="36"/>
       <c r="B14" t="s">
         <v>817</v>
       </c>
@@ -22574,7 +22574,7 @@
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="32"/>
+      <c r="A15" s="36"/>
       <c r="B15" t="s">
         <v>821</v>
       </c>
@@ -22602,7 +22602,7 @@
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="32"/>
+      <c r="A16" s="36"/>
       <c r="B16" t="s">
         <v>819</v>
       </c>
@@ -22630,7 +22630,7 @@
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="32"/>
+      <c r="A17" s="36"/>
       <c r="B17" t="s">
         <v>863</v>
       </c>
@@ -22658,7 +22658,7 @@
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="32"/>
+      <c r="A18" s="36"/>
       <c r="B18" t="s">
         <v>864</v>
       </c>
@@ -22686,7 +22686,7 @@
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="32"/>
+      <c r="A19" s="36"/>
       <c r="B19" t="s">
         <v>818</v>
       </c>
@@ -22694,14 +22694,14 @@
         <v>17</v>
       </c>
       <c r="D19" s="19">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E19" s="19">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F19" s="20">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="G19" s="20" t="s">
         <v>883</v>
@@ -22710,11 +22710,11 @@
         <v>794</v>
       </c>
       <c r="I19" s="26" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="32"/>
+      <c r="A20" s="36"/>
       <c r="B20" t="s">
         <v>820</v>
       </c>
@@ -22725,11 +22725,11 @@
         <v>16</v>
       </c>
       <c r="E20" s="19">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F20" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="G20" s="20" t="s">
         <v>829</v>
@@ -22742,7 +22742,7 @@
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="32"/>
+      <c r="A21" s="36"/>
       <c r="B21" t="s">
         <v>865</v>
       </c>
@@ -22770,7 +22770,7 @@
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="32"/>
+      <c r="A22" s="36"/>
       <c r="B22" t="s">
         <v>825</v>
       </c>
@@ -22798,7 +22798,7 @@
       </c>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="32"/>
+      <c r="A23" s="36"/>
       <c r="B23" t="s">
         <v>826</v>
       </c>
@@ -22809,11 +22809,11 @@
         <v>15</v>
       </c>
       <c r="E23" s="19">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F23" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G23" s="20" t="s">
         <v>883</v>
@@ -22822,11 +22822,11 @@
         <v>866</v>
       </c>
       <c r="I23" s="26" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="32"/>
+      <c r="A24" s="36"/>
       <c r="B24" t="s">
         <v>827</v>
       </c>
@@ -22854,7 +22854,7 @@
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="32"/>
+      <c r="A25" s="36"/>
       <c r="B25" t="s">
         <v>823</v>
       </c>
@@ -22882,20 +22882,20 @@
       </c>
     </row>
     <row r="26" spans="1:9">
-      <c r="B26" s="34"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="36">
+      <c r="B26" s="30"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="32">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G26" s="36"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="37"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="33"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>891</v>
       </c>
       <c r="B27" t="s">
@@ -22916,7 +22916,7 @@
       </c>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="31"/>
+      <c r="A28" s="37"/>
       <c r="B28" t="s">
         <v>838</v>
       </c>
@@ -22935,7 +22935,7 @@
       </c>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="31"/>
+      <c r="A29" s="37"/>
       <c r="B29" t="s">
         <v>840</v>
       </c>
@@ -22954,14 +22954,16 @@
       </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="31"/>
+      <c r="A30" s="37"/>
       <c r="B30" s="21" t="s">
         <v>836</v>
       </c>
       <c r="C30" s="19">
         <v>293</v>
       </c>
-      <c r="D30" s="20"/>
+      <c r="D30" s="20">
+        <v>104</v>
+      </c>
       <c r="E30" s="20"/>
       <c r="F30" s="20">
         <f>IF(AND(D30=0,D30&lt;&gt;""),100,IF(ISERROR(E30/D30*100),0,ROUNDUP(E30/D30 * 100, 0)))</f>
@@ -22978,7 +22980,7 @@
       </c>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="31"/>
+      <c r="A31" s="37"/>
       <c r="B31" t="s">
         <v>843</v>
       </c>
@@ -22997,7 +22999,7 @@
       </c>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="31"/>
+      <c r="A32" s="37"/>
       <c r="B32" t="s">
         <v>839</v>
       </c>
@@ -23013,7 +23015,7 @@
       </c>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="31"/>
+      <c r="A33" s="37"/>
       <c r="B33" t="s">
         <v>841</v>
       </c>
@@ -23029,7 +23031,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="28">
-      <c r="A34" s="31"/>
+      <c r="A34" s="37"/>
       <c r="B34" t="s">
         <v>842</v>
       </c>
@@ -23045,7 +23047,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="28">
-      <c r="A35" s="31"/>
+      <c r="A35" s="37"/>
       <c r="B35" t="s">
         <v>844</v>
       </c>
@@ -23061,7 +23063,7 @@
       </c>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="31"/>
+      <c r="A36" s="37"/>
       <c r="B36" t="s">
         <v>845</v>
       </c>
@@ -23077,7 +23079,7 @@
       </c>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="31"/>
+      <c r="A37" s="37"/>
       <c r="B37" t="s">
         <v>846</v>
       </c>
@@ -23093,7 +23095,7 @@
       </c>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="31"/>
+      <c r="A38" s="37"/>
       <c r="B38" t="s">
         <v>623</v>
       </c>
@@ -23109,7 +23111,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="28">
-      <c r="A39" s="31"/>
+      <c r="A39" s="37"/>
       <c r="B39" t="s">
         <v>847</v>
       </c>
@@ -23125,7 +23127,7 @@
       </c>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="31"/>
+      <c r="A40" s="37"/>
       <c r="B40" t="s">
         <v>881</v>
       </c>
@@ -23141,7 +23143,7 @@
       </c>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="31"/>
+      <c r="A41" s="37"/>
       <c r="B41" t="s">
         <v>824</v>
       </c>
@@ -23149,7 +23151,7 @@
         <v>52</v>
       </c>
       <c r="F41" s="20">
-        <f>IF(AND(D41=0,D41&lt;&gt;""),100,IF(ISERROR(E41/D41*100),0,ROUNDUP(E41/D41 * 100, 0)))</f>
+        <f t="shared" ref="F41:F46" si="2">IF(AND(D41=0,D41&lt;&gt;""),100,IF(ISERROR(E41/D41*100),0,ROUNDUP(E41/D41 * 100, 0)))</f>
         <v>0</v>
       </c>
       <c r="G41" s="20" t="s">
@@ -23160,7 +23162,7 @@
       </c>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="31"/>
+      <c r="A42" s="37"/>
       <c r="B42" t="s">
         <v>878</v>
       </c>
@@ -23168,7 +23170,7 @@
         <v>38</v>
       </c>
       <c r="F42" s="25">
-        <f>IF(AND(D42=0,D42&lt;&gt;""),100,IF(ISERROR(E42/D42*100),0,ROUNDUP(E42/D42 * 100, 0)))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G42" s="25" t="s">
@@ -23179,7 +23181,7 @@
       </c>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="31"/>
+      <c r="A43" s="37"/>
       <c r="B43" t="s">
         <v>15</v>
       </c>
@@ -23187,7 +23189,7 @@
         <v>22</v>
       </c>
       <c r="F43" s="25">
-        <f>IF(AND(D43=0,D43&lt;&gt;""),100,IF(ISERROR(E43/D43*100),0,ROUNDUP(E43/D43 * 100, 0)))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G43" s="25" t="s">
@@ -23198,7 +23200,7 @@
       </c>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="31"/>
+      <c r="A44" s="37"/>
       <c r="B44" t="s">
         <v>822</v>
       </c>
@@ -23206,7 +23208,7 @@
         <v>20</v>
       </c>
       <c r="F44" s="20">
-        <f>IF(AND(D44=0,D44&lt;&gt;""),100,IF(ISERROR(E44/D44*100),0,ROUNDUP(E44/D44 * 100, 0)))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G44" s="20" t="s">
@@ -23217,7 +23219,7 @@
       </c>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="31"/>
+      <c r="A45" s="37"/>
       <c r="B45" t="s">
         <v>860</v>
       </c>
@@ -23225,7 +23227,7 @@
         <v>81</v>
       </c>
       <c r="F45" s="20">
-        <f>IF(AND(D45=0,D45&lt;&gt;""),100,IF(ISERROR(E45/D45*100),0,ROUNDUP(E45/D45 * 100, 0)))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G45" s="20" t="s">
@@ -23236,7 +23238,7 @@
       </c>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="31"/>
+      <c r="A46" s="37"/>
       <c r="B46" t="s">
         <v>861</v>
       </c>
@@ -23244,7 +23246,7 @@
         <v>177</v>
       </c>
       <c r="F46" s="20">
-        <f>IF(AND(D46=0,D46&lt;&gt;""),100,IF(ISERROR(E46/D46*100),0,ROUNDUP(E46/D46 * 100, 0)))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G46" s="20" t="s">
@@ -23255,20 +23257,20 @@
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="B47" s="34"/>
-      <c r="C47" s="35"/>
-      <c r="D47" s="35"/>
-      <c r="E47" s="35"/>
-      <c r="F47" s="36">
+      <c r="B47" s="30"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="32">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G47" s="36"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="37"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="31"/>
+      <c r="I47" s="33"/>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="33" t="s">
+      <c r="A48" s="35" t="s">
         <v>892</v>
       </c>
       <c r="B48" t="s">
@@ -23286,7 +23288,7 @@
       </c>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="33"/>
+      <c r="A49" s="35"/>
       <c r="B49" t="s">
         <v>849</v>
       </c>
@@ -23302,7 +23304,7 @@
       </c>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="33"/>
+      <c r="A50" s="35"/>
       <c r="B50" t="s">
         <v>850</v>
       </c>
@@ -23316,7 +23318,7 @@
       <c r="G50" s="20"/>
     </row>
     <row r="51" spans="1:9">
-      <c r="A51" s="33"/>
+      <c r="A51" s="35"/>
       <c r="B51" t="s">
         <v>851</v>
       </c>
@@ -23330,7 +23332,7 @@
       <c r="G51" s="20"/>
     </row>
     <row r="52" spans="1:9">
-      <c r="A52" s="33"/>
+      <c r="A52" s="35"/>
       <c r="B52" t="s">
         <v>852</v>
       </c>
@@ -23344,7 +23346,7 @@
       <c r="G52" s="20"/>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="33"/>
+      <c r="A53" s="35"/>
       <c r="B53" t="s">
         <v>853</v>
       </c>
@@ -23358,7 +23360,7 @@
       <c r="G53" s="20"/>
     </row>
     <row r="54" spans="1:9">
-      <c r="A54" s="33"/>
+      <c r="A54" s="35"/>
       <c r="B54" t="s">
         <v>854</v>
       </c>
@@ -23372,7 +23374,7 @@
       <c r="G54" s="20"/>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="33"/>
+      <c r="A55" s="35"/>
       <c r="B55" t="s">
         <v>855</v>
       </c>
@@ -23386,7 +23388,7 @@
       <c r="G55" s="20"/>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="33"/>
+      <c r="A56" s="35"/>
       <c r="B56" t="s">
         <v>747</v>
       </c>
@@ -23401,17 +23403,17 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="19"/>
-      <c r="B57" s="34"/>
-      <c r="C57" s="35"/>
-      <c r="D57" s="35"/>
-      <c r="E57" s="35"/>
-      <c r="F57" s="36">
+      <c r="B57" s="30"/>
+      <c r="C57" s="31"/>
+      <c r="D57" s="31"/>
+      <c r="E57" s="31"/>
+      <c r="F57" s="32">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G57" s="36"/>
-      <c r="H57" s="35"/>
-      <c r="I57" s="37"/>
+      <c r="G57" s="32"/>
+      <c r="H57" s="31"/>
+      <c r="I57" s="33"/>
     </row>
     <row r="58" spans="1:9" ht="15" thickBot="1">
       <c r="A58" s="19" t="s">
@@ -23436,15 +23438,15 @@
       </c>
       <c r="D59" s="23">
         <f>SUM(Table13[Automation Candidate '#])</f>
-        <v>420</v>
+        <v>526</v>
       </c>
       <c r="E59" s="23">
         <f>SUM(Table13[Automated Case '#])</f>
-        <v>265</v>
+        <v>295</v>
       </c>
       <c r="F59" s="24">
         <f>ROUNDUP(E59/D59 * 100, 0)</f>
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="G59" s="24"/>
       <c r="H59" s="23"/>

</xml_diff>

<commit_message>
1. Update current automation status 2. Update rand() method to be back compatable with ruby1.9.2. Tested in QA6 build 2.4.0.17
Change-Id: I3bd1fd1d789b5dbc13fe2e737993acc753cc9fe3
Reviewed-on: https://gerrit.dechocorp.com/48290
Reviewed-by: Kalen Quam <kquam@vmware.com>
Reviewed-by: Spark Yao <shipuy@mozy.com>
</commit_message>
<xml_diff>
--- a/automation_tracking.xlsx
+++ b/automation_tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16620" activeTab="4"/>
+    <workbookView xWindow="29040" yWindow="-1680" windowWidth="28800" windowHeight="16620" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="4" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4244" uniqueCount="894">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4248" uniqueCount="897">
   <si>
     <t>Billing Automation Test Plan</t>
   </si>
@@ -2735,9 +2735,6 @@
     <t>Neale clean up cases in progress</t>
   </si>
   <si>
-    <t>Cleaning up cases</t>
-  </si>
-  <si>
     <t>Smoke Test (for production)</t>
   </si>
   <si>
@@ -2775,6 +2772,18 @@
   </si>
   <si>
     <t>IV</t>
+  </si>
+  <si>
+    <t>Clean up Target Date 3/29/2013</t>
+  </si>
+  <si>
+    <t>Clean up Target Date 3/15/2013</t>
+  </si>
+  <si>
+    <t>Clean up Target Date 3/22/2013</t>
+  </si>
+  <si>
+    <t>Clean up Target Date 4/5/2013</t>
   </si>
 </sst>
 </file>
@@ -22189,7 +22198,7 @@
   <dimension ref="A2:I59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -22201,14 +22210,14 @@
     <col min="6" max="6" width="15.83203125" style="19" customWidth="1"/>
     <col min="7" max="7" width="9.5" style="28" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.83203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.33203125" style="26" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="29" thickBot="1">
       <c r="A2" s="29" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>830</v>
@@ -22226,7 +22235,7 @@
         <v>869</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="H2" s="20" t="s">
         <v>876</v>
@@ -22237,7 +22246,7 @@
     </row>
     <row r="3" spans="1:9" ht="15" thickTop="1">
       <c r="A3" s="36" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>831</v>
@@ -22704,7 +22713,7 @@
         <v>100</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="H19" s="19" t="s">
         <v>794</v>
@@ -22760,7 +22769,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="H21" s="19" t="s">
         <v>829</v>
@@ -22788,7 +22797,7 @@
         <v>15</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="H22" s="19" t="s">
         <v>866</v>
@@ -22816,7 +22825,7 @@
         <v>100</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="H23" s="19" t="s">
         <v>866</v>
@@ -22844,7 +22853,7 @@
         <v>0</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="H24" s="19" t="s">
         <v>829</v>
@@ -22896,7 +22905,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="37" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="B27" t="s">
         <v>837</v>
@@ -22909,10 +22918,13 @@
         <v>0</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>829</v>
+        <v>794</v>
       </c>
       <c r="H27" s="19" t="s">
-        <v>829</v>
+        <v>794</v>
+      </c>
+      <c r="I27" s="26" t="s">
+        <v>893</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -22933,6 +22945,9 @@
       <c r="H28" s="19" t="s">
         <v>829</v>
       </c>
+      <c r="I28" s="26" t="s">
+        <v>894</v>
+      </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="37"/>
@@ -22947,10 +22962,13 @@
         <v>0</v>
       </c>
       <c r="G29" s="20" t="s">
-        <v>829</v>
+        <v>866</v>
       </c>
       <c r="H29" s="19" t="s">
-        <v>829</v>
+        <v>866</v>
+      </c>
+      <c r="I29" s="26" t="s">
+        <v>895</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -22964,10 +22982,12 @@
       <c r="D30" s="20">
         <v>104</v>
       </c>
-      <c r="E30" s="20"/>
+      <c r="E30" s="20">
+        <v>24</v>
+      </c>
       <c r="F30" s="20">
         <f>IF(AND(D30=0,D30&lt;&gt;""),100,IF(ISERROR(E30/D30*100),0,ROUNDUP(E30/D30 * 100, 0)))</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="G30" s="20" t="s">
         <v>794</v>
@@ -22976,7 +22996,7 @@
         <v>794</v>
       </c>
       <c r="I30" s="19" t="s">
-        <v>880</v>
+        <v>873</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -22992,10 +23012,13 @@
         <v>0</v>
       </c>
       <c r="G31" s="20" t="s">
-        <v>829</v>
+        <v>866</v>
       </c>
       <c r="H31" s="19" t="s">
-        <v>829</v>
+        <v>866</v>
+      </c>
+      <c r="I31" s="26" t="s">
+        <v>896</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -23011,7 +23034,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -23027,7 +23050,7 @@
         <v>0</v>
       </c>
       <c r="G33" s="20" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="28">
@@ -23043,7 +23066,7 @@
         <v>0</v>
       </c>
       <c r="G34" s="20" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="28">
@@ -23059,7 +23082,7 @@
         <v>0</v>
       </c>
       <c r="G35" s="20" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -23075,7 +23098,7 @@
         <v>0</v>
       </c>
       <c r="G36" s="20" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -23123,13 +23146,13 @@
         <v>0</v>
       </c>
       <c r="G39" s="20" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="37"/>
       <c r="B40" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="C40" s="19">
         <v>12</v>
@@ -23139,7 +23162,7 @@
         <v>0</v>
       </c>
       <c r="G40" s="25" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -23155,7 +23178,7 @@
         <v>0</v>
       </c>
       <c r="G41" s="20" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="I41" s="26" t="s">
         <v>875</v>
@@ -23174,7 +23197,7 @@
         <v>0</v>
       </c>
       <c r="G42" s="25" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="I42" s="26" t="s">
         <v>875</v>
@@ -23193,7 +23216,7 @@
         <v>0</v>
       </c>
       <c r="G43" s="25" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="I43" s="26" t="s">
         <v>879</v>
@@ -23212,7 +23235,7 @@
         <v>0</v>
       </c>
       <c r="G44" s="20" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="I44" s="19" t="s">
         <v>879</v>
@@ -23271,7 +23294,7 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="35" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="B48" t="s">
         <v>848</v>
@@ -23284,7 +23307,7 @@
         <v>0</v>
       </c>
       <c r="G48" s="20" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -23300,7 +23323,7 @@
         <v>0</v>
       </c>
       <c r="G49" s="20" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -23417,7 +23440,7 @@
     </row>
     <row r="58" spans="1:9" ht="15" thickBot="1">
       <c r="A58" s="19" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="C58" s="19">
         <v>1929</v>
@@ -23442,11 +23465,11 @@
       </c>
       <c r="E59" s="23">
         <f>SUM(Table13[Automated Case '#])</f>
-        <v>295</v>
+        <v>319</v>
       </c>
       <c r="F59" s="24">
         <f>ROUNDUP(E59/D59 * 100, 0)</f>
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G59" s="24"/>
       <c r="H59" s="23"/>

</xml_diff>